<commit_message>
registration and login done
</commit_message>
<xml_diff>
--- a/registration_details.xlsx
+++ b/registration_details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" state="visible" r:id="rId1"/>
@@ -423,8 +423,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -470,32 +470,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>r230014</t>
+          <t>r230014@famt.ac.in</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>r230014@famt.ac.in</t>
+          <t>Samiya</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Samiya Khalid Akhatar Budye</t>
+          <t>$2b$12$J55QWV5Dai8.x34A7o9lwufpgAhn/4oWgfrFuPZtc2idJVDFJL25C</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>student</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>saamia.kb@gmail.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>$2b$12$NGK9X3gne.ZNkNhE9RdkyOwEBpucto3t7M3P46fIo5i2/R0g2pni6</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>student</t>
         </is>
       </c>
     </row>
@@ -512,7 +507,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>